<commit_message>
Vista Registeration Scenarios completed, Dated:25052024
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data.xlsx
+++ b/src/test/resources/test-data.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\eclipse-workspace\page-object-framework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ShariqueA\OneDrive - AXA\Documents\Automation-Personal\VistaAutomation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A112EACD-FED2-4EB7-B427-AFE10E8089F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{656E41A6-CB0A-46A3-A4CC-80945889B007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{CDFF5931-B191-4B97-BBD5-1BF9BE3326AF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CDFF5931-B191-4B97-BBD5-1BF9BE3326AF}"/>
   </bookViews>
   <sheets>
-    <sheet name="login_credentials" sheetId="1" r:id="rId1"/>
+    <sheet name="Login" sheetId="2" r:id="rId1"/>
+    <sheet name="Registeration" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,28 +26,114 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>userId</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>mngr571718</t>
-  </si>
-  <si>
-    <t>patygYh</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="28">
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>EmailId</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>BirthDate</t>
+  </si>
+  <si>
+    <t>OffersChebox</t>
+  </si>
+  <si>
+    <t>TermsCheckbox</t>
+  </si>
+  <si>
+    <t>NewsletterCheckbox</t>
+  </si>
+  <si>
+    <t>DataPrivacyCheckbox</t>
+  </si>
+  <si>
+    <t>ScenarioType</t>
+  </si>
+  <si>
+    <t>Positive</t>
+  </si>
+  <si>
+    <t>Mr</t>
+  </si>
+  <si>
+    <t>Testhnnj</t>
+  </si>
+  <si>
+    <t>Uhnnkkk</t>
+  </si>
+  <si>
+    <t>05/15/1986</t>
+  </si>
+  <si>
+    <t>Negative</t>
+  </si>
+  <si>
+    <t>ScenarioId</t>
+  </si>
+  <si>
+    <t>RegisterationScenario1</t>
+  </si>
+  <si>
+    <t>RegisterationScenario2</t>
+  </si>
+  <si>
+    <t>SocialTitle</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>TesthnnjUhnnkkk1716664676120@test.com</t>
+  </si>
+  <si>
+    <t>TesthnnjUhnnkkk1236</t>
+  </si>
+  <si>
+    <t>RegisterationScenario3</t>
+  </si>
+  <si>
+    <t>RegisterationScenario4</t>
+  </si>
+  <si>
+    <t>RegisterationScenario5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -69,13 +156,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -387,33 +480,312 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD2E5C89-673F-476D-BC24-27CCEC594163}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6476698E-4588-4A1A-86B5-781D421E21A4}">
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{91FAA2FA-F643-41AE-8D8D-EE776A4CC108}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{F6A8BA80-4041-4C4C-81AD-F87863616A84}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD2E5C89-673F-476D-BC24-27CCEC594163}">
+  <dimension ref="A1:K6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1" t="str">
+        <f>CONCATENATE(D2,E2,1236)</f>
+        <v>TesthnnjUhnnkkk1236</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1" t="str">
+        <f>CONCATENATE(D3,E3,1236)</f>
+        <v>TesthnnjUhnnkkk1236</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="1" t="str">
+        <f t="shared" ref="F4:F5" si="0">CONCATENATE(D4,E4,1236)</f>
+        <v>TesthnnjUhnnkkk1236</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>TesthnnjUhnnkkk1236</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Login Scenarios Dated 26052024
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data.xlsx
+++ b/src/test/resources/test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ShariqueA\OneDrive - AXA\Documents\Automation-Personal\VistaAutomation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{656E41A6-CB0A-46A3-A4CC-80945889B007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4573576-157E-4742-A8A6-08850EE6FC4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CDFF5931-B191-4B97-BBD5-1BF9BE3326AF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CDFF5931-B191-4B97-BBD5-1BF9BE3326AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="32">
   <si>
     <t>FirstName</t>
   </si>
@@ -110,6 +110,18 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>jgjhgkkllklKL997000</t>
+  </si>
+  <si>
+    <t>LoginScenario1</t>
+  </si>
+  <si>
+    <t>LoginScenario2</t>
+  </si>
+  <si>
+    <t>LoginScenario3</t>
   </si>
 </sst>
 </file>
@@ -160,12 +172,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -481,18 +498,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6476698E-4588-4A1A-86B5-781D421E21A4}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -502,45 +520,61 @@
       <c r="B1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D3" t="s">
-        <v>23</v>
+      <c r="D3" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{91FAA2FA-F643-41AE-8D8D-EE776A4CC108}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{F6A8BA80-4041-4C4C-81AD-F87863616A84}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{22A9099F-7A6F-479F-9597-8D6446AC9F3B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -550,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD2E5C89-673F-476D-BC24-27CCEC594163}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Initiating Shopping Scenarios Dated:26 May 2024
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data.xlsx
+++ b/src/test/resources/test-data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ShariqueA\OneDrive - AXA\Documents\Automation-Personal\VistaAutomation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4573576-157E-4742-A8A6-08850EE6FC4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310E7373-F043-402D-B52D-8960F9B9E3BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CDFF5931-B191-4B97-BBD5-1BF9BE3326AF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{CDFF5931-B191-4B97-BBD5-1BF9BE3326AF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Login" sheetId="2" r:id="rId1"/>
-    <sheet name="Registeration" sheetId="1" r:id="rId2"/>
+    <sheet name="Registeration" sheetId="1" r:id="rId1"/>
+    <sheet name="Login" sheetId="2" r:id="rId2"/>
+    <sheet name="Shoping" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -497,95 +498,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6476698E-4588-4A1A-86B5-781D421E21A4}">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{91FAA2FA-F643-41AE-8D8D-EE776A4CC108}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{F6A8BA80-4041-4C4C-81AD-F87863616A84}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{22A9099F-7A6F-479F-9597-8D6446AC9F3B}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD2E5C89-673F-476D-BC24-27CCEC594163}">
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,4 +739,102 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6476698E-4588-4A1A-86B5-781D421E21A4}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{91FAA2FA-F643-41AE-8D8D-EE776A4CC108}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{F6A8BA80-4041-4C4C-81AD-F87863616A84}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{22A9099F-7A6F-479F-9597-8D6446AC9F3B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FBEE27F-1CD5-415B-95F2-E2B4E0E772C3}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Shopping Method, Dated: 27 May 2024
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data.xlsx
+++ b/src/test/resources/test-data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ShariqueA\OneDrive - AXA\Documents\Automation-Personal\VistaAutomation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310E7373-F043-402D-B52D-8960F9B9E3BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9768F7EA-3AC5-454E-BC28-4EF0719162FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{CDFF5931-B191-4B97-BBD5-1BF9BE3326AF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CDFF5931-B191-4B97-BBD5-1BF9BE3326AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Registeration" sheetId="1" r:id="rId1"/>
     <sheet name="Login" sheetId="2" r:id="rId2"/>
     <sheet name="Shoping" sheetId="3" r:id="rId3"/>
+    <sheet name="DropDownMappingSheet" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="61">
   <si>
     <t>FirstName</t>
   </si>
@@ -123,6 +124,93 @@
   </si>
   <si>
     <t>LoginScenario3</t>
+  </si>
+  <si>
+    <t>Clothes</t>
+  </si>
+  <si>
+    <t>Men</t>
+  </si>
+  <si>
+    <t>Women</t>
+  </si>
+  <si>
+    <t>Accessories</t>
+  </si>
+  <si>
+    <t>Home Accessories</t>
+  </si>
+  <si>
+    <t>Art</t>
+  </si>
+  <si>
+    <t>ShoppingScenario1</t>
+  </si>
+  <si>
+    <t>ProductCategory</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>ProductPrice</t>
+  </si>
+  <si>
+    <t>Hummingbird printed t-shirt</t>
+  </si>
+  <si>
+    <t>$23.90</t>
+  </si>
+  <si>
+    <t>ShoppingScenario2</t>
+  </si>
+  <si>
+    <t>ShoppingScenario3</t>
+  </si>
+  <si>
+    <t>ShoppingScenario4</t>
+  </si>
+  <si>
+    <t>ShoppingScenario5</t>
+  </si>
+  <si>
+    <t>$35.90</t>
+  </si>
+  <si>
+    <t>Hummingbird printed sweater</t>
+  </si>
+  <si>
+    <t>Brown bear notebook</t>
+  </si>
+  <si>
+    <t>$12.90</t>
+  </si>
+  <si>
+    <t>Mountain fox cushion</t>
+  </si>
+  <si>
+    <t>$18.90</t>
+  </si>
+  <si>
+    <t>Brown bear - Vector graphics</t>
+  </si>
+  <si>
+    <t>$9.00</t>
+  </si>
+  <si>
+    <t>PaymentOption</t>
+  </si>
+  <si>
+    <t>MenuOption</t>
+  </si>
+  <si>
+    <t>ps_wirepayment</t>
+  </si>
+  <si>
+    <t>ps_checkpayment</t>
+  </si>
+  <si>
+    <t>ps_cashondelivery</t>
   </si>
 </sst>
 </file>
@@ -160,11 +248,40 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -173,7 +290,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -184,12 +301,81 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -200,6 +386,16 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{854D02C9-A0F9-428B-BAF3-216A6C97A978}" name="PaymentOption" displayName="PaymentOption" ref="A1:A4" totalsRowShown="0" headerRowDxfId="5" dataDxfId="3" headerRowBorderDxfId="4" tableBorderDxfId="2" totalsRowBorderDxfId="1">
+  <autoFilter ref="A1:A4" xr:uid="{854D02C9-A0F9-428B-BAF3-216A6C97A978}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{673D552E-C16F-49C3-B5B0-14118AE35483}" name="PaymentOption" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -502,7 +698,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="H2" sqref="H2:K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,10 +939,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6476698E-4588-4A1A-86B5-781D421E21A4}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -814,12 +1010,27 @@
         <v>28</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{91FAA2FA-F643-41AE-8D8D-EE776A4CC108}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{F6A8BA80-4041-4C4C-81AD-F87863616A84}"/>
     <hyperlink ref="C4" r:id="rId3" xr:uid="{22A9099F-7A6F-479F-9597-8D6446AC9F3B}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{DEFA68B2-A06A-4394-89C5-8BC2AAB9D550}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -827,14 +1038,216 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FBEE27F-1CD5-415B-95F2-E2B4E0E772C3}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D6" xr:uid="{D26C43CD-3593-4ED3-94A3-A14581341390}">
+      <formula1>"Men,Women,Accessories,Home Accessories,Art"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C6" xr:uid="{79851F51-F035-4272-A314-B1FA5627A45B}">
+      <formula1>"Clothes, Accessories,Art"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G6" xr:uid="{BD52C8F1-EF1C-4ECA-850D-BEA6ADCB626E}">
+      <formula1>INDIRECT("PaymentOption[PaymentOption]")</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DF2662B-D102-41E8-BE22-8BD61223ADB2}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Shopping Scenarios & Started Listener & Retry Concept Dated: 28 May 2024
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data.xlsx
+++ b/src/test/resources/test-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ShariqueA\OneDrive - AXA\Documents\Automation-Personal\VistaAutomation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9768F7EA-3AC5-454E-BC28-4EF0719162FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B959AEBB-87BF-420A-BF47-693BB5FD5D8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CDFF5931-B191-4B97-BBD5-1BF9BE3326AF}"/>
   </bookViews>
@@ -942,7 +942,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:D5"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1041,7 +1041,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add SQL Connection Logic Dated 09 June 2024
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data.xlsx
+++ b/src/test/resources/test-data.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ShariqueA\OneDrive - AXA\Documents\Automation-Personal\VistaAutomation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B959AEBB-87BF-420A-BF47-693BB5FD5D8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF776EB9-026E-41DC-9CE1-51F729FB9451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CDFF5931-B191-4B97-BBD5-1BF9BE3326AF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CDFF5931-B191-4B97-BBD5-1BF9BE3326AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Registeration" sheetId="1" r:id="rId1"/>
     <sheet name="Login" sheetId="2" r:id="rId2"/>
-    <sheet name="Shoping" sheetId="3" r:id="rId3"/>
+    <sheet name="Shopping" sheetId="3" r:id="rId3"/>
     <sheet name="DropDownMappingSheet" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -697,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD2E5C89-673F-476D-BC24-27CCEC594163}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:K6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,7 +941,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6476698E-4588-4A1A-86B5-781D421E21A4}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
@@ -1041,7 +1041,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>